<commit_message>
Unprotected Excel sheets while in development
</commit_message>
<xml_diff>
--- a/BulkUploadTemplate.xlsx
+++ b/BulkUploadTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccarthy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Master\MvpApi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="7965" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Enter Your Data Here" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
   <si>
     <t>Blog Site Posts</t>
   </si>
@@ -618,7 +618,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="AwardCategoryNames" displayName="AwardCategoryNames" ref="A1:A19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:A19"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="AwardCategory" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" uniqueName="1" name="AwardCategory" queryTableFieldId="1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,7 +628,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ContributionTypes" displayName="ContributionTypes" ref="A1:A26" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:A26"/>
   <tableColumns count="1">
-    <tableColumn id="1" uniqueName="1" name="ContributionType" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" uniqueName="1" name="ContributionType" queryTableFieldId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -931,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,29 +947,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1100,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="H+wXOqMU9jRmjmV27s2v6d2Td1pBFfhfSOb9fsoip36ImsOPfXBNb0DJWTu40OfP7Kl5khd5F4R8GjDc0ciofQ==" saltValue="bDCaEjdEhBbabMAvAXvbXQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1123,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
@@ -1553,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1693,7 +1682,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8eaexy0iieHvbg4tUa40M3pG109YTPovEjGqZZG+JajyfAUgbw3HbrOhNDD4IjMokYqSVe4hfPnwNO0BD+jB4Q==" saltValue="lYxS3FzJbMJ3eYoZe7GEIA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed typo in Excel Template's validation error messge
</commit_message>
<xml_diff>
--- a/BulkUploadTemplate.xlsx
+++ b/BulkUploadTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="7965" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Enter Your Data Here" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>Blog Site Posts</t>
   </si>
@@ -933,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,15 +950,18 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -979,7 +982,7 @@
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="You need to choose from th elist of items in the dropdown." promptTitle="Select an Award Category" prompt="Choose from the list of award categories in the drop down.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="You must choose one of the award categories listed in the drop down." promptTitle="Select an Award Category" prompt="Choose from the list of award categories in the drop down.">
           <x14:formula1>
             <xm:f>ReadOnly_AwardCategories!$A$2:$A$19</xm:f>
           </x14:formula1>
@@ -1542,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Excel doc's DataValidation logic! Confirmed suggestion from @dsdalg in #10 works!
</commit_message>
<xml_diff>
--- a/BulkUploadTemplate.xlsx
+++ b/BulkUploadTemplate.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="140">
   <si>
     <t>Blog Site Posts</t>
   </si>
@@ -934,14 +934,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -950,10 +950,10 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -963,12 +963,18 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select a Category Technology" prompt="The list of available technologies in the drop down are dependent on the previously selected Award Category." sqref="C1:C1048576">
-      <formula1>INDIRECT($B:$B)</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invlaid Entry" error="This cell must contain one of the values from the drop down list." promptTitle="Pick Technology" prompt="Choose from your award categories available technologies." sqref="C1">
+      <formula1>INDIRECT(SUBSTITUTE(B1," ","_"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>INDIRECT(SUBSTITUTE(B2," ","_"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1115,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>

</xml_diff>